<commit_message>
Add Tests for Traceability Matrix
</commit_message>
<xml_diff>
--- a/code/cov_tool/output/EXAMPLE/EX_TEST_param_trace.xlsx
+++ b/code/cov_tool/output/EXAMPLE/EX_TEST_param_trace.xlsx
@@ -52,7 +52,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -108,6 +108,39 @@
       <top style="thin">
         <color rgb="00000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="00000000"/>
       </bottom>
@@ -491,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,46 +533,46 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Object</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Transitions</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Transitions</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>States</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
@@ -551,6 +584,11 @@
           <t>Sequencer</t>
         </is>
       </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>Object</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -558,42 +596,94 @@
           <t>Multiple</t>
         </is>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Multiple</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="D4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="4" t="n">
-        <v>1</v>
+      <c r="E4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" s="3" t="n"/>
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="n">
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Multiple</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="n">
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n"/>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
+  <mergeCells count="4">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>